<commit_message>
add new change from server
</commit_message>
<xml_diff>
--- a/excel_files/Assets_A.xlsx
+++ b/excel_files/Assets_A.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,6 +509,21 @@
           <t>parent_permid</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>projectimage</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>authoritytocreate</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Company_Name</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -572,6 +587,9 @@
       <c r="O2" t="n">
         <v>5000030092</v>
       </c>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -637,6 +655,9 @@
       <c r="O3" t="n">
         <v>5000030092</v>
       </c>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -702,6 +723,9 @@
       <c r="O4" t="n">
         <v>5000030092</v>
       </c>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -765,6 +789,9 @@
       <c r="O5" t="n">
         <v>5000030092</v>
       </c>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -830,6 +857,9 @@
       <c r="O6" t="n">
         <v>5000030092</v>
       </c>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -895,6 +925,9 @@
       <c r="O7" t="n">
         <v>5000030092</v>
       </c>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -958,6 +991,9 @@
       <c r="O8" t="n">
         <v>5000030092</v>
       </c>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1021,6 +1057,9 @@
       <c r="O9" t="n">
         <v>5000030092</v>
       </c>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1084,6 +1123,161 @@
       <c r="O10" t="n">
         <v>5000030092</v>
       </c>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ArcelorMittal SA sonu</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>GASTBEL0009</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Flémalle</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Wallonie</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Belgium</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>BEL</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>56</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Europe</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Western Europe</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>50.594707</v>
+      </c>
+      <c r="K11" t="n">
+        <v>5.466776</v>
+      </c>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="n">
+        <v>5000060650</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>ArcelorMittal Belgium SA sonu</t>
+        </is>
+      </c>
+      <c r="O11" t="n">
+        <v>5000030093</v>
+      </c>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>""</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>""</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Archiologist</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Dallas</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>New York</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>1234521</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>40.92679582427576</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>-94.53104228055014</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>Arcel</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="n">
+        <v>1</v>
+      </c>
+      <c r="R13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>